<commit_message>
update_offer_agg - first successful run (tbd: several offers complete at same point in time)
</commit_message>
<xml_diff>
--- a/data/offer_agg.xlsx
+++ b/data/offer_agg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://porsche-my.sharepoint.com/personal/oliver_balb_porsche_de/Documents/Documents/_Orga/96 - Training/DataScience/05 CapStone/Starbucks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_08B51184DD79720E6235547658CD2E3BA8039430" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBDBDB16-4191-4D13-B0E3-CEE5748AA543}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_08B51184DD79720E6235547658CD2E3BA8039430" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2A625E2-D562-4D47-B12E-B9477CAA3DE3}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -488,7 +487,7 @@
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
@@ -519,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -545,7 +544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -571,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -597,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1393</v>
       </c>
@@ -649,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>54574</v>
       </c>
@@ -701,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>112214</v>
       </c>
@@ -727,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>150598</v>
       </c>
@@ -753,7 +752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>150600</v>
       </c>
@@ -779,7 +778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>152030</v>
       </c>
@@ -805,7 +804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>201572</v>
       </c>
@@ -831,7 +830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>201573</v>
       </c>
@@ -857,7 +856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>201574</v>
       </c>
@@ -883,7 +882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>202962</v>
       </c>
@@ -909,7 +908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>245125</v>
       </c>
@@ -935,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>246495</v>
       </c>
@@ -962,13 +961,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H18" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2eeac8d8feae4a8cad5a6af0499a211d"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>